<commit_message>
Generación de archivo fisico
</commit_message>
<xml_diff>
--- a/input/reporte_transacciones_16-10-2025_15-08-42.xlsx
+++ b/input/reporte_transacciones_16-10-2025_15-08-42.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="104">
   <si>
     <t>País</t>
   </si>
@@ -261,9 +261,6 @@
     <t>2025-09-30T15:15:58-03:00</t>
   </si>
   <si>
-    <t>FAILED</t>
-  </si>
-  <si>
     <t>AMEX</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
   </si>
   <si>
     <t>2025-10-01T17:11:31-03:00</t>
-  </si>
-  <si>
-    <t>REJECTED</t>
   </si>
   <si>
     <t>CUOTA_SIMPLE</t>
@@ -372,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -388,6 +382,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1403,7 +1400,7 @@
         <v>80</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="M6" s="1">
         <v>105.24</v>
@@ -1415,16 +1412,16 @@
         <v>48</v>
       </c>
       <c r="P6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="T6" s="2">
         <v>1.0</v>
@@ -1508,7 +1505,7 @@
         <v>65</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
@@ -1537,16 +1534,16 @@
         <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="M7" s="2">
         <v>1.2345678925E8</v>
@@ -1648,10 +1645,10 @@
         <v>48</v>
       </c>
       <c r="AT7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8">
@@ -1680,19 +1677,19 @@
         <v>51</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M8" s="1">
-        <v>100.0</v>
+        <v>54</v>
+      </c>
+      <c r="M8" s="2">
+        <v>40008.54</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>48</v>
@@ -1710,7 +1707,7 @@
         <v>48</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T8" s="2">
         <v>1.0</v>
@@ -1791,7 +1788,7 @@
         <v>48</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU8" s="1" t="s">
         <v>66</v>
@@ -1823,16 +1820,16 @@
         <v>51</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>48</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="M9" s="5">
         <v>150.02</v>
@@ -1853,7 +1850,7 @@
         <v>48</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T9" s="3" t="s">
         <v>71</v>
@@ -1934,7 +1931,7 @@
         <v>48</v>
       </c>
       <c r="AT9" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU9" s="3" t="s">
         <v>66</v>
@@ -1966,19 +1963,19 @@
         <v>51</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>48</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="5">
-        <v>100.0</v>
+      <c r="M10" s="6">
+        <v>16846.35</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>48</v>
@@ -1990,7 +1987,7 @@
         <v>55</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R10" s="5">
         <v>0.0</v>
@@ -2023,7 +2020,7 @@
         <v>90.83</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AC10" s="3" t="s">
         <v>61</v>
@@ -2056,7 +2053,7 @@
         <v>81.81</v>
       </c>
       <c r="AM10" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AN10" s="3" t="s">
         <v>64</v>
@@ -2077,7 +2074,7 @@
         <v>2.97</v>
       </c>
       <c r="AT10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU10" s="3" t="s">
         <v>66</v>
@@ -2109,19 +2106,19 @@
         <v>51</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>48</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="L11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M11" s="5">
-        <v>100.0</v>
+      <c r="M11" s="6">
+        <v>1111235.55</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>48</v>
@@ -2142,7 +2139,7 @@
         <v>70</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>59</v>
@@ -2166,7 +2163,7 @@
         <v>82.81</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AC11" s="3" t="s">
         <v>61</v>
@@ -2199,7 +2196,7 @@
         <v>74.07</v>
       </c>
       <c r="AM11" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AN11" s="3" t="s">
         <v>64</v>
@@ -2220,7 +2217,7 @@
         <v>2.69</v>
       </c>
       <c r="AT11" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU11" s="3" t="s">
         <v>66</v>
@@ -2252,16 +2249,16 @@
         <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="M12" s="1">
         <v>150.02</v>
@@ -2282,7 +2279,7 @@
         <v>48</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>71</v>
@@ -2363,7 +2360,7 @@
         <v>48</v>
       </c>
       <c r="AT12" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU12" s="1" t="s">
         <v>66</v>
@@ -2395,19 +2392,19 @@
         <v>51</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="1">
-        <v>100.0</v>
+      <c r="M13" s="2">
+        <v>115.25</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>48</v>
@@ -2419,7 +2416,7 @@
         <v>55</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R13" s="1">
         <v>0.0</v>
@@ -2452,7 +2449,7 @@
         <v>90.83</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AC13" s="1" t="s">
         <v>61</v>
@@ -2485,7 +2482,7 @@
         <v>81.81</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AN13" s="1" t="s">
         <v>64</v>
@@ -2506,7 +2503,7 @@
         <v>2.97</v>
       </c>
       <c r="AT13" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU13" s="1" t="s">
         <v>66</v>
@@ -2538,19 +2535,19 @@
         <v>51</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M14" s="1">
-        <v>100.0</v>
+      <c r="M14" s="2">
+        <v>130.48</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>48</v>
@@ -2571,7 +2568,7 @@
         <v>70</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>59</v>
@@ -2595,7 +2592,7 @@
         <v>82.81</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AC14" s="1" t="s">
         <v>61</v>
@@ -2628,7 +2625,7 @@
         <v>74.07</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AN14" s="1" t="s">
         <v>64</v>
@@ -2649,7 +2646,7 @@
         <v>2.69</v>
       </c>
       <c r="AT14" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AU14" s="1" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
comento descarga de archivos en archivosdiarios.php
</commit_message>
<xml_diff>
--- a/input/reporte_transacciones_16-10-2025_15-08-42.xlsx
+++ b/input/reporte_transacciones_16-10-2025_15-08-42.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="105">
   <si>
     <t>País</t>
   </si>
@@ -162,22 +162,25 @@
     <t>morellinicolas7@gmail.com</t>
   </si>
   <si>
+    <t>C11672</t>
+  </si>
+  <si>
+    <t>CUIT</t>
+  </si>
+  <si>
+    <t>30717440885</t>
+  </si>
+  <si>
+    <t>PAYMENT</t>
+  </si>
+  <si>
+    <t>37226978</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>CUIT</t>
-  </si>
-  <si>
-    <t>30717440885</t>
-  </si>
-  <si>
-    <t>PAYMENT</t>
-  </si>
-  <si>
-    <t>37226978</t>
-  </si>
-  <si>
-    <t>2025-09-30T15:12:07-03:00</t>
+    <t>2025-10-15T15:12:07-03:00</t>
   </si>
   <si>
     <t>APPROVED</t>
@@ -222,7 +225,7 @@
     <t>952927789</t>
   </si>
   <si>
-    <t>2025-09-30T15:13:07-03:00</t>
+    <t>2025-10-15T15:13:07-03:00</t>
   </si>
   <si>
     <t>CREDIT</t>
@@ -243,7 +246,7 @@
     <t>622917540</t>
   </si>
   <si>
-    <t>2025-09-30T15:13:51-03:00</t>
+    <t>2025-10-15T15:13:51-03:00</t>
   </si>
   <si>
     <t>PREPAID</t>
@@ -252,13 +255,13 @@
     <t>515349427</t>
   </si>
   <si>
-    <t>2025-09-30T15:15:17-03:00</t>
+    <t>2025-10-15T15:15:17-03:00</t>
   </si>
   <si>
     <t>65682583</t>
   </si>
   <si>
-    <t>2025-09-30T15:15:58-03:00</t>
+    <t>2025-10-15T15:15:58-03:00</t>
   </si>
   <si>
     <t>AMEX</t>
@@ -276,7 +279,7 @@
     <t>472632866</t>
   </si>
   <si>
-    <t>2025-10-01T17:11:31-03:00</t>
+    <t>2025-10-15T17:11:31-03:00</t>
   </si>
   <si>
     <t>CUOTA_SIMPLE</t>
@@ -288,7 +291,7 @@
     <t>762471688</t>
   </si>
   <si>
-    <t>2025-10-01T17:12:23-03:00</t>
+    <t>2025-10-15T17:12:23-03:00</t>
   </si>
   <si>
     <t>XXXXXXXXXXXX4129</t>
@@ -297,13 +300,13 @@
     <t>192861357</t>
   </si>
   <si>
-    <t>2025-10-19T17:14:20-03:00</t>
+    <t>2025-10-15T17:14:20-03:00</t>
   </si>
   <si>
     <t>799676995</t>
   </si>
   <si>
-    <t>2025-10-19T17:32:08-03:00</t>
+    <t>2025-10-15T17:32:08-03:00</t>
   </si>
   <si>
     <t>2025-10-15</t>
@@ -315,7 +318,7 @@
     <t>173946229</t>
   </si>
   <si>
-    <t>2025-10-18T17:32:45-03:00</t>
+    <t>2025-10-15T17:32:45-03:00</t>
   </si>
   <si>
     <t>6</t>
@@ -806,7 +809,7 @@
       <c r="D2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -822,40 +825,40 @@
         <v>52</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>53</v>
+        <v>53</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M2" s="1">
         <v>100.0</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R2" s="1">
         <v>0.0</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V2" s="1">
         <v>0.0</v>
@@ -876,13 +879,13 @@
         <v>100.0</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AE2" s="1">
         <v>3.0</v>
@@ -909,10 +912,10 @@
         <v>93.0</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO2" s="1">
         <v>0.35</v>
@@ -930,10 +933,10 @@
         <v>3.37</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -949,7 +952,7 @@
       <c r="D3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -962,43 +965,43 @@
         <v>51</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>68</v>
+        <v>53</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M3" s="1">
         <v>120.25</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R3" s="1">
         <v>0.0</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V3" s="1">
         <v>13.92</v>
@@ -1019,13 +1022,13 @@
         <v>100.0</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE3" s="1">
         <v>5.0</v>
@@ -1052,10 +1055,10 @@
         <v>89.48</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO3" s="1">
         <v>0.35</v>
@@ -1073,10 +1076,10 @@
         <v>3.25</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4">
@@ -1092,7 +1095,7 @@
       <c r="D4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1105,43 +1108,43 @@
         <v>51</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M4" s="1">
         <v>138.36</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R4" s="1">
         <v>0.0</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T4" s="2">
         <v>1.0</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V4" s="1">
         <v>22.91</v>
@@ -1162,13 +1165,13 @@
         <v>100.0</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE4" s="1">
         <v>5.0</v>
@@ -1195,10 +1198,10 @@
         <v>88.42</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO4" s="1">
         <v>0.35</v>
@@ -1216,10 +1219,10 @@
         <v>3.21</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
@@ -1235,7 +1238,7 @@
       <c r="D5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1248,43 +1251,43 @@
         <v>51</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>78</v>
+        <v>53</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M5" s="1">
         <v>105.23</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R5" s="1">
         <v>0.0</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T5" s="2">
         <v>1.0</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V5" s="1">
         <v>13.92</v>
@@ -1305,13 +1308,13 @@
         <v>87.51</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE5" s="1">
         <v>5.0</v>
@@ -1338,10 +1341,10 @@
         <v>78.31</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO5" s="1">
         <v>0.35</v>
@@ -1359,10 +1362,10 @@
         <v>2.84</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
@@ -1378,7 +1381,7 @@
       <c r="D6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -1391,121 +1394,121 @@
         <v>51</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M6" s="1">
         <v>105.24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="T6" s="2">
         <v>1.0</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AS6" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
@@ -1521,7 +1524,7 @@
       <c r="D7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -1534,121 +1537,121 @@
         <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>86</v>
+        <v>53</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M7" s="2">
         <v>1.2345678925E8</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T7" s="2">
         <v>2.0</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AJ7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AL7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AM7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AP7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AQ7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AR7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AS7" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AT7" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -1664,7 +1667,7 @@
       <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -1677,121 +1680,121 @@
         <v>51</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>90</v>
+        <v>53</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M8" s="2">
         <v>40008.54</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T8" s="2">
         <v>1.0</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AJ8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AK8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AM8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AP8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AQ8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AR8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AS8" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AT8" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU8" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
@@ -1807,7 +1810,7 @@
       <c r="D9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1820,121 +1823,121 @@
         <v>51</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M9" s="5">
         <v>150.02</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AG9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AH9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AK9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AL9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AM9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AN9" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AP9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AQ9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AR9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AS9" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AT9" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU9" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10">
@@ -1950,7 +1953,7 @@
       <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1963,43 +1966,43 @@
         <v>51</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M10" s="6">
         <v>16846.35</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R10" s="5">
         <v>0.0</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T10" s="5">
         <v>1.0</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V10" s="5">
         <v>7.58</v>
@@ -2020,13 +2023,13 @@
         <v>90.83</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD10" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE10" s="5">
         <v>5.0</v>
@@ -2053,10 +2056,10 @@
         <v>81.81</v>
       </c>
       <c r="AM10" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AN10" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO10" s="5">
         <v>0.35</v>
@@ -2074,10 +2077,10 @@
         <v>2.97</v>
       </c>
       <c r="AT10" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU10" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
@@ -2093,7 +2096,7 @@
       <c r="D11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -2106,43 +2109,43 @@
         <v>51</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M11" s="6">
         <v>1111235.55</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R11" s="5">
         <v>0.0</v>
       </c>
       <c r="S11" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V11" s="5">
         <v>14.21</v>
@@ -2163,13 +2166,13 @@
         <v>82.81</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD11" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE11" s="5">
         <v>5.0</v>
@@ -2196,10 +2199,10 @@
         <v>74.07</v>
       </c>
       <c r="AM11" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO11" s="5">
         <v>0.35</v>
@@ -2217,10 +2220,10 @@
         <v>2.69</v>
       </c>
       <c r="AT11" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU11" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
@@ -2236,7 +2239,7 @@
       <c r="D12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -2249,121 +2252,121 @@
         <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M12" s="1">
         <v>150.02</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AJ12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AL12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AM12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AN12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AP12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AQ12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AR12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AS12" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="AT12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU12" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13">
@@ -2379,7 +2382,7 @@
       <c r="D13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -2392,43 +2395,43 @@
         <v>51</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M13" s="2">
         <v>115.25</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R13" s="1">
         <v>0.0</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T13" s="2">
         <v>1.0</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V13" s="1">
         <v>7.58</v>
@@ -2449,13 +2452,13 @@
         <v>90.83</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE13" s="1">
         <v>5.0</v>
@@ -2482,10 +2485,10 @@
         <v>81.81</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO13" s="1">
         <v>0.35</v>
@@ -2503,10 +2506,10 @@
         <v>2.97</v>
       </c>
       <c r="AT13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
@@ -2522,7 +2525,7 @@
       <c r="D14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -2535,43 +2538,43 @@
         <v>51</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M14" s="2">
         <v>130.48</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R14" s="1">
         <v>0.0</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V14" s="1">
         <v>14.21</v>
@@ -2592,13 +2595,13 @@
         <v>82.81</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AE14" s="1">
         <v>5.0</v>
@@ -2625,10 +2628,10 @@
         <v>74.07</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AN14" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AO14" s="1">
         <v>0.35</v>
@@ -2646,10 +2649,10 @@
         <v>2.69</v>
       </c>
       <c r="AT14" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AU14" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1"/>

</xml_diff>